<commit_message>
tidied up H2O-CO2 benchmark.
</commit_message>
<xml_diff>
--- a/Benchmarking/COS_H2O_EOS_DZ2006/KerrickJacobs81_Density-Pressure-Calc.xlsx
+++ b/Benchmarking/COS_H2O_EOS_DZ2006/KerrickJacobs81_Density-Pressure-Calc.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akluegel/AK_Data/Mikrothermometrie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\Box\Berkeley_new\DiadFit_outer\Benchmarking\COS_H2O_EOS_DZ2006\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D00516-E964-394C-9EDA-D5F6FA9F1066}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48525D17-C22B-4001-B65F-A7EFEF646BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="1740" windowWidth="32740" windowHeight="19740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="250" windowWidth="19190" windowHeight="10070" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pure CO2" sheetId="1" r:id="rId1"/>
     <sheet name="0.9 CO2 + 0.1 H2O" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1631,14 +1644,14 @@
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1649,7 +1662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0.51300000000000001</v>
       </c>
@@ -1661,7 +1674,7 @@
         <v>230.56650037943572</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.59499999999999997</v>
       </c>
@@ -1673,7 +1686,7 @@
         <v>288.43833676703537</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.63100000000000001</v>
       </c>
@@ -1685,7 +1698,7 @@
         <v>318.23729835163584</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.65600000000000003</v>
       </c>
@@ -1697,7 +1710,7 @@
         <v>340.7238501959647</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>0.67700000000000005</v>
       </c>
@@ -1709,7 +1722,7 @@
         <v>360.83591493135248</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>0.69499999999999995</v>
       </c>
@@ -1721,7 +1734,7 @@
         <v>379.01710111013705</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>0.71099999999999997</v>
       </c>
@@ -1733,7 +1746,7 @@
         <v>395.94579704104433</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>0.72599999999999998</v>
       </c>
@@ -1745,7 +1758,7 @@
         <v>412.50252448807737</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>0.73899999999999999</v>
       </c>
@@ -1757,7 +1770,7 @@
         <v>427.41067780007592</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>0.752</v>
       </c>
@@ -1769,7 +1782,7 @@
         <v>442.8576230514692</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>0.76300000000000001</v>
       </c>
@@ -1781,7 +1794,7 @@
         <v>456.36335608329512</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>0.77400000000000002</v>
       </c>
@@ -1793,7 +1806,7 @@
         <v>470.2809705308008</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>0.78500000000000003</v>
       </c>
@@ -1805,7 +1818,7 @@
         <v>484.62302745232944</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>0.79400000000000004</v>
       </c>
@@ -1817,7 +1830,7 @@
         <v>496.68217058498254</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>0.80400000000000005</v>
       </c>
@@ -1829,7 +1842,7 @@
         <v>510.43348012073722</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>0.81299999999999994</v>
       </c>
@@ -1841,7 +1854,7 @@
         <v>523.13487903864075</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>0.82199999999999995</v>
       </c>
@@ -1853,7 +1866,7 @@
         <v>536.15233389870843</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>0.83</v>
       </c>
@@ -1865,7 +1878,7 @@
         <v>547.99508927294448</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>0.83799999999999997</v>
       </c>
@@ -1877,7 +1890,7 @@
         <v>560.09943234527725</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>0.84599999999999997</v>
       </c>
@@ -1889,7 +1902,7 @@
         <v>572.47114117340027</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>0.85399999999999998</v>
       </c>
@@ -1901,7 +1914,7 @@
         <v>585.11612144314415</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>0.86199999999999999</v>
       </c>
@@ -1913,7 +1926,7 @@
         <v>598.04040928757956</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>0.92800000000000005</v>
       </c>
@@ -1925,7 +1938,7 @@
         <v>716.16051566661019</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>0.98299999999999998</v>
       </c>
@@ -1937,7 +1950,7 @@
         <v>832.23040013739444</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>1.032</v>
       </c>
@@ -1949,7 +1962,7 @@
         <v>951.39404589952983</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>1.0760000000000001</v>
       </c>
@@ -1961,7 +1974,7 @@
         <v>1072.8697275712425</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>1.117</v>
       </c>
@@ -1973,7 +1986,7 @@
         <v>1199.9837880507287</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>1.155</v>
       </c>
@@ -1999,17 +2012,17 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2020,7 +2033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0.1</v>
       </c>
@@ -2032,7 +2045,7 @@
         <v>28.994450000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.15</v>
       </c>
@@ -2044,7 +2057,7 @@
         <v>48.308706249999993</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.2</v>
       </c>
@@ -2056,7 +2069,7 @@
         <v>68.201599999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.25</v>
       </c>
@@ -2068,7 +2081,7 @@
         <v>89.25209375</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>0.3</v>
       </c>
@@ -2080,7 +2093,7 @@
         <v>112.03914999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>0.35</v>
       </c>
@@ -2092,7 +2105,7 @@
         <v>137.14173124999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>0.4</v>
       </c>
@@ -2104,7 +2117,7 @@
         <v>165.1388</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>0.45</v>
       </c>
@@ -2116,7 +2129,7 @@
         <v>196.60931875</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>0.5</v>
       </c>
@@ -2128,7 +2141,7 @@
         <v>232.13225</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>0.55000000000000004</v>
       </c>
@@ -2140,7 +2153,7 @@
         <v>272.28655625000005</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>0.6</v>
       </c>
@@ -2152,7 +2165,7 @@
         <v>317.65119999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>0.65</v>
       </c>
@@ -2164,7 +2177,7 @@
         <v>368.80514375000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>0.7</v>
       </c>
@@ -2176,7 +2189,7 @@
         <v>426.32734999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>0.75</v>
       </c>
@@ -2188,7 +2201,7 @@
         <v>490.79678125000004</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>0.8</v>
       </c>
@@ -2200,7 +2213,7 @@
         <v>562.79240000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>0.85</v>
       </c>
@@ -2212,52 +2225,52 @@
         <v>642.89316874999997</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="5"/>
     </row>
   </sheetData>

</xml_diff>